<commit_message>
atualizacao para as avaliacoes e correcao
</commit_message>
<xml_diff>
--- a/src/analises/result/excel/mefs_aleatorias/fsm_random-all_results.xlsx
+++ b/src/analises/result/excel/mefs_aleatorias/fsm_random-all_results.xlsx
@@ -1,29 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matheus/eclipse-workspace/H-SwitchCover/src/analises/result/excel/mefs_aleatorias/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E00D7B-6781-4649-B96A-88487A84D8A1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2567C1E0-E0E4-0D41-B422-C2B821696C29}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14420" yWindow="460" windowWidth="23640" windowHeight="19520" xr2:uid="{2EE634F3-C8F3-7B4E-B54A-B04D9C0D3C86}"/>
+    <workbookView xWindow="14980" yWindow="460" windowWidth="23060" windowHeight="19520" xr2:uid="{2EE634F3-C8F3-7B4E-B54A-B04D9C0D3C86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$23</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$33</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$4:$A$12</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$R$24:$R$32</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$R$34:$R$42</definedName>
-  </definedNames>
-  <calcPr calcId="179021"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -423,19 +415,19 @@
                   <c:v>25.41237113</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29.979797980000001</c:v>
+                  <c:v>29.838383839999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35.848484849999998</c:v>
+                  <c:v>35.505050509999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41.74</c:v>
+                  <c:v>41.32</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>47.175257729999998</c:v>
+                  <c:v>46.804123709999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>53.103092779999997</c:v>
+                  <c:v>52.793814429999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -539,19 +531,19 @@
                   <c:v>9.5670103090000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.56565657</c:v>
+                  <c:v>11.51515152</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.070707069999999</c:v>
+                  <c:v>14.020202019999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.43</c:v>
+                  <c:v>16.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.24742268</c:v>
+                  <c:v>18.18556701</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20.40206186</c:v>
+                  <c:v>20.30927835</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1189,31 +1181,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>564.47474750000003</c:v>
+                  <c:v>2249.1414140000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1335.9285709999999</c:v>
+                  <c:v>5308.3979589999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2362.083333</c:v>
+                  <c:v>9403.4270830000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3802.6494849999999</c:v>
+                  <c:v>15126.329900000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5478.181818</c:v>
+                  <c:v>21825.686870000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7488.7474750000001</c:v>
+                  <c:v>29916.545450000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9726.83</c:v>
+                  <c:v>38953.08</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12308.804120000001</c:v>
+                  <c:v>49206.164949999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15198.144329999999</c:v>
+                  <c:v>60834.75258</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1856,31 +1848,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>546.71717169999999</c:v>
+                  <c:v>2178.6161619999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1307.887755</c:v>
+                  <c:v>5197.1122450000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2322.041667</c:v>
+                  <c:v>9243.6145830000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3753.2268039999999</c:v>
+                  <c:v>14928.94845</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5417.30303</c:v>
+                  <c:v>21582.888889999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7415.8383839999997</c:v>
+                  <c:v>29625.373739999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9641.89</c:v>
+                  <c:v>38613.72</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12215.268040000001</c:v>
+                  <c:v>48832.041239999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15095.37113</c:v>
+                  <c:v>60424.010309999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2528,31 +2520,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>16.171717170000001</c:v>
+                  <c:v>12.212121209999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.132653059999999</c:v>
+                  <c:v>14.64285714</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.208333329999999</c:v>
+                  <c:v>16.208333329999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.391752579999999</c:v>
+                  <c:v>19.824742270000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.272727270000001</c:v>
+                  <c:v>20.979797980000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.929292929999999</c:v>
+                  <c:v>20.272727270000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26.72</c:v>
+                  <c:v>17.77</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29.515463919999998</c:v>
+                  <c:v>21.958762889999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30.618556699999999</c:v>
+                  <c:v>23.298969069999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3190,31 +3182,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>42.18181818</c:v>
+                  <c:v>43.19191919</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63.306122449999997</c:v>
+                  <c:v>64.908163270000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>79.75</c:v>
+                  <c:v>81.322916669999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>99.030927840000004</c:v>
+                  <c:v>100.8659794</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>116.1010101</c:v>
+                  <c:v>118.01010100000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>134.05050510000001</c:v>
+                  <c:v>135.969697</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>149.53</c:v>
+                  <c:v>151.80000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>170.57731960000001</c:v>
+                  <c:v>172.56701029999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>190.5257732</c:v>
+                  <c:v>193.19587630000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3852,31 +3844,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>31.917368079999999</c:v>
+                  <c:v>31.843807160000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.346883339999998</c:v>
+                  <c:v>48.435101549999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60.11468919</c:v>
+                  <c:v>60.082717520000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>78.284567550000006</c:v>
+                  <c:v>77.986594100000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>91.332784939999996</c:v>
+                  <c:v>91.190876320000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>103.4549698</c:v>
+                  <c:v>103.54163389999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>115.5809029</c:v>
+                  <c:v>115.82207440000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>132.63237570000001</c:v>
+                  <c:v>132.50407939999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>148.90385570000001</c:v>
+                  <c:v>149.11104280000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4514,31 +4506,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>8.2257861139999999</c:v>
+                  <c:v>8.3447393939999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.25976197</c:v>
+                  <c:v>13.319270319999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.91002361</c:v>
+                  <c:v>16.98016702</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.011952409999999</c:v>
+                  <c:v>20.336356469999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.707913600000001</c:v>
+                  <c:v>23.809413370000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29.003534940000002</c:v>
+                  <c:v>28.87701839</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.858662119999998</c:v>
+                  <c:v>33.603654380000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>37.083239519999999</c:v>
+                  <c:v>37.05771867</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41.944222099999998</c:v>
+                  <c:v>41.5851288</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5176,31 +5168,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>78.766284540000001</c:v>
+                  <c:v>79.043439520000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>190.4274882</c:v>
+                  <c:v>190.68622719999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>309.77868050000001</c:v>
+                  <c:v>308.86185360000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>434.67973760000001</c:v>
+                  <c:v>447.93002239999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>605.69968159999996</c:v>
+                  <c:v>607.16225970000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>897.39863620000006</c:v>
+                  <c:v>884.43729010000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1227.8741</c:v>
+                  <c:v>1199.4864789999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1428.062895</c:v>
+                  <c:v>1424.5244849999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1845.465841</c:v>
+                  <c:v>1801.413258</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7045,19 +7037,19 @@
                   <c:v>135.43298970000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>191.45454549999999</c:v>
+                  <c:v>171.0909091</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>253.91919189999999</c:v>
+                  <c:v>210.26262629999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>324</c:v>
+                  <c:v>252.12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>392.1443299</c:v>
+                  <c:v>295.9072165</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>471.32989689999999</c:v>
+                  <c:v>344.60824739999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7161,19 +7153,19 @@
                   <c:v>219.4948454</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>356.18181820000001</c:v>
+                  <c:v>307.49494950000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>528.08080810000001</c:v>
+                  <c:v>414.97979800000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>749.47</c:v>
+                  <c:v>543.62</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>987.86597940000001</c:v>
+                  <c:v>692.65979379999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1256.639175</c:v>
+                  <c:v>846.8556701</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7272,19 +7264,19 @@
                   <c:v>297.94845359999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>413.22222219999998</c:v>
+                  <c:v>351.68686869999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>468.71717169999999</c:v>
+                  <c:v>368.93939390000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>549.33000000000004</c:v>
+                  <c:v>401.67</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>613.0927835</c:v>
+                  <c:v>425.39175260000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>665.18556699999999</c:v>
+                  <c:v>437.63917529999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7388,19 +7380,19 @@
                   <c:v>54.731958759999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>76.424242419999999</c:v>
+                  <c:v>65.646464649999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>98.686868689999997</c:v>
+                  <c:v>76.858585860000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>121.93</c:v>
+                  <c:v>88.94</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>141.8247423</c:v>
+                  <c:v>99.175257729999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>162.95876290000001</c:v>
+                  <c:v>109.0103093</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9872,19 +9864,19 @@
                   <c:v>110.02061860000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>161.47474750000001</c:v>
+                  <c:v>141.2525253</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>218.07070709999999</c:v>
+                  <c:v>174.75757580000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>282.26</c:v>
+                  <c:v>210.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>344.96907220000003</c:v>
+                  <c:v>249.10309280000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>418.22680409999998</c:v>
+                  <c:v>291.81443300000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9988,19 +9980,19 @@
                   <c:v>209.92783510000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>344.6161616</c:v>
+                  <c:v>295.97979800000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>514.01010099999996</c:v>
+                  <c:v>400.95959599999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>733.04</c:v>
+                  <c:v>527.32000000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>969.6185567</c:v>
+                  <c:v>674.4742268</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1236.2371129999999</c:v>
+                  <c:v>826.54639180000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10099,19 +10091,19 @@
                   <c:v>296.94845359999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>412.22222219999998</c:v>
+                  <c:v>350.68686869999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>467.71717169999999</c:v>
+                  <c:v>367.93939390000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>548.33000000000004</c:v>
+                  <c:v>400.67</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>612.0927835</c:v>
+                  <c:v>424.39175260000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>664.18556699999999</c:v>
+                  <c:v>436.63917529999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10215,19 +10207,19 @@
                   <c:v>53.731958759999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>75.424242419999999</c:v>
+                  <c:v>64.646464649999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>97.686868689999997</c:v>
+                  <c:v>75.858585860000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>120.93</c:v>
+                  <c:v>87.94</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>140.8247423</c:v>
+                  <c:v>98.175257729999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>161.95876290000001</c:v>
+                  <c:v>108.0103093</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10539,19 +10531,19 @@
                   <c:v>2.3298969070000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3535353539999999</c:v>
+                  <c:v>2.3030303029999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.4444444440000002</c:v>
+                  <c:v>2.2929292929999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.54</c:v>
+                  <c:v>2.27</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.6391752579999999</c:v>
+                  <c:v>2.3402061860000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.628865979</c:v>
+                  <c:v>2.3195876289999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10655,19 +10647,19 @@
                   <c:v>15.29896907</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.28282828</c:v>
+                  <c:v>15.919191919999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.01010101</c:v>
+                  <c:v>15.969696969999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23.75</c:v>
+                  <c:v>17.21</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27</c:v>
+                  <c:v>19.18556701</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29.15463918</c:v>
+                  <c:v>20.051546389999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10766,19 +10758,19 @@
                   <c:v>296.94845359999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>412.22222219999998</c:v>
+                  <c:v>350.68686869999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>467.71717169999999</c:v>
+                  <c:v>367.93939390000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>548.33000000000004</c:v>
+                  <c:v>400.67</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>612.0927835</c:v>
+                  <c:v>424.39175260000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>664.18556699999999</c:v>
+                  <c:v>436.63917529999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10882,19 +10874,19 @@
                   <c:v>53.731958759999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>75.424242419999999</c:v>
+                  <c:v>64.646464649999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>97.686868689999997</c:v>
+                  <c:v>75.858585860000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>120.93</c:v>
+                  <c:v>87.94</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>140.8247423</c:v>
+                  <c:v>98.175257729999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>161.95876290000001</c:v>
+                  <c:v>108.0103093</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11206,19 +11198,19 @@
                   <c:v>6.0515463919999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.5858585860000005</c:v>
+                  <c:v>6.9191919190000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.848484848</c:v>
+                  <c:v>7.3131313130000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.03</c:v>
+                  <c:v>7.69</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.48453608</c:v>
+                  <c:v>8.2474226799999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.42268041</c:v>
+                  <c:v>8.7525773200000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11322,19 +11314,19 @@
                   <c:v>28.226804120000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.939393940000002</c:v>
+                  <c:v>33.272727269999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>47.777777780000001</c:v>
+                  <c:v>37.171717170000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>58.66</c:v>
+                  <c:v>42.38</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>69.18556701</c:v>
+                  <c:v>47.927835049999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>79.12371134</c:v>
+                  <c:v>52.886597940000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11433,19 +11425,19 @@
                   <c:v>296.94845359999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>412.22222219999998</c:v>
+                  <c:v>350.68686869999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>467.71717169999999</c:v>
+                  <c:v>367.93939390000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>548.33000000000004</c:v>
+                  <c:v>400.67</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>612.0927835</c:v>
+                  <c:v>424.39175260000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>664.18556699999999</c:v>
+                  <c:v>436.63917529999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11549,19 +11541,19 @@
                   <c:v>53.731958759999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>75.424242419999999</c:v>
+                  <c:v>64.646464649999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>97.686868689999997</c:v>
+                  <c:v>75.858585860000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>120.93</c:v>
+                  <c:v>87.94</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>140.8247423</c:v>
+                  <c:v>98.175257729999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>161.95876290000001</c:v>
+                  <c:v>108.0103093</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11878,19 +11870,19 @@
                   <c:v>4.3298289250000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.3951768700000002</c:v>
+                  <c:v>4.7433795249999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0935587680000003</c:v>
+                  <c:v>4.9297355119999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.7648798040000004</c:v>
+                  <c:v>5.1034099060000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.3057515039999998</c:v>
+                  <c:v>5.321230226</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.8820218970000004</c:v>
+                  <c:v>5.5314001839999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11994,19 +11986,19 @@
                   <c:v>22.69553496</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.427251779999999</c:v>
+                  <c:v>26.213870579999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.322766270000002</c:v>
+                  <c:v>29.209199430000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45.74794953</c:v>
+                  <c:v>33.14454963</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>54.054142400000003</c:v>
+                  <c:v>37.70811621</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>61.604193250000002</c:v>
+                  <c:v>41.392901979999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12105,19 +12097,19 @@
                   <c:v>296.94845359999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>412.22222219999998</c:v>
+                  <c:v>350.68686869999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>467.71717169999999</c:v>
+                  <c:v>367.93939390000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>548.33000000000004</c:v>
+                  <c:v>400.67</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>612.0927835</c:v>
+                  <c:v>424.39175260000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>664.18556699999999</c:v>
+                  <c:v>436.63917529999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12221,19 +12213,19 @@
                   <c:v>53.731958759999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>75.424242419999999</c:v>
+                  <c:v>64.646464649999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>97.686868689999997</c:v>
+                  <c:v>75.858585860000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>120.93</c:v>
+                  <c:v>87.94</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>140.8247423</c:v>
+                  <c:v>98.175257729999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>161.95876290000001</c:v>
+                  <c:v>108.0103093</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12540,19 +12532,19 @@
                   <c:v>1.163039261</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.7335318159999999</c:v>
+                  <c:v>1.3717702380000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.026309758</c:v>
+                  <c:v>1.460244136</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3153459949999999</c:v>
+                  <c:v>1.532455846</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.6335990909999998</c:v>
+                  <c:v>1.6476098530000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.8838130820000001</c:v>
+                  <c:v>1.7880565479999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12656,19 +12648,19 @@
                   <c:v>4.8284088159999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.4665058220000002</c:v>
+                  <c:v>6.3452085580000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.3793808120000008</c:v>
+                  <c:v>7.2011670309999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.76933337</c:v>
+                  <c:v>8.5527159229999992</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.684280660000001</c:v>
+                  <c:v>9.3981537530000008</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.86573351</c:v>
+                  <c:v>10.517408469999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13202,19 +13194,19 @@
                   <c:v>1.482662903</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.2653379820000001</c:v>
+                  <c:v>2.0713742740000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.5257334440000001</c:v>
+                  <c:v>2.3759268699999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.8435752550000002</c:v>
+                  <c:v>2.5594885889999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.6195127749999996</c:v>
+                  <c:v>3.02126677</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0837061119999998</c:v>
+                  <c:v>3.538067093</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13318,19 +13310,19 @@
                   <c:v>30.252994170000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70.172124819999993</c:v>
+                  <c:v>50.763472829999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>103.10665</c:v>
+                  <c:v>60.436836079999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>166.5898833</c:v>
+                  <c:v>88.030601090000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>213.8925749</c:v>
+                  <c:v>100.1391471</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>281.54371459999999</c:v>
+                  <c:v>123.91606470000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13968,31 +13960,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>17.757575760000002</c:v>
+                  <c:v>70.525252530000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.040816329999998</c:v>
+                  <c:v>111.2857143</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40.041666669999998</c:v>
+                  <c:v>159.8125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49.422680409999998</c:v>
+                  <c:v>197.3814433</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60.878787879999997</c:v>
+                  <c:v>242.79797980000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72.909090910000003</c:v>
+                  <c:v>291.17171719999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>84.94</c:v>
+                  <c:v>339.36</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>93.536082469999997</c:v>
+                  <c:v>374.12371130000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>102.7731959</c:v>
+                  <c:v>410.74226800000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -22207,8 +22199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27355D29-B019-1441-9750-10D890D0A95F}">
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L170" workbookViewId="0">
-      <selection activeCell="M211" sqref="M211"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34:R42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22534,28 +22526,28 @@
         <v>12</v>
       </c>
       <c r="B8" s="1">
-        <v>29.979797980000001</v>
+        <v>29.838383839999999</v>
       </c>
       <c r="C8" s="1">
-        <v>191.45454549999999</v>
+        <v>171.0909091</v>
       </c>
       <c r="D8" s="1">
-        <v>161.47474750000001</v>
+        <v>141.2525253</v>
       </c>
       <c r="E8" s="1">
-        <v>2.3535353539999999</v>
+        <v>2.3030303029999999</v>
       </c>
       <c r="F8" s="1">
-        <v>8.5858585860000005</v>
+        <v>6.9191919190000002</v>
       </c>
       <c r="G8" s="1">
-        <v>5.3951768700000002</v>
+        <v>4.7433795249999999</v>
       </c>
       <c r="H8" s="1">
-        <v>1.7335318159999999</v>
+        <v>1.3717702380000001</v>
       </c>
       <c r="I8" s="1">
-        <v>3.2653379820000001</v>
+        <v>2.0713742740000001</v>
       </c>
       <c r="K8" s="1">
         <v>580</v>
@@ -22587,28 +22579,28 @@
         <v>14</v>
       </c>
       <c r="B9" s="8">
-        <v>35.848484849999998</v>
+        <v>35.505050509999997</v>
       </c>
       <c r="C9" s="8">
-        <v>253.91919189999999</v>
+        <v>210.26262629999999</v>
       </c>
       <c r="D9" s="8">
-        <v>218.07070709999999</v>
+        <v>174.75757580000001</v>
       </c>
       <c r="E9" s="8">
-        <v>2.4444444440000002</v>
+        <v>2.2929292929999998</v>
       </c>
       <c r="F9" s="8">
-        <v>9.848484848</v>
+        <v>7.3131313130000004</v>
       </c>
       <c r="G9" s="8">
-        <v>6.0935587680000003</v>
+        <v>4.9297355119999997</v>
       </c>
       <c r="H9" s="8">
-        <v>2.026309758</v>
+        <v>1.460244136</v>
       </c>
       <c r="I9" s="8">
-        <v>4.5257334440000001</v>
+        <v>2.3759268699999998</v>
       </c>
       <c r="K9" s="8">
         <v>676</v>
@@ -22640,28 +22632,28 @@
         <v>16</v>
       </c>
       <c r="B10" s="1">
-        <v>41.74</v>
+        <v>41.32</v>
       </c>
       <c r="C10" s="1">
-        <v>324</v>
+        <v>252.12</v>
       </c>
       <c r="D10" s="1">
-        <v>282.26</v>
+        <v>210.8</v>
       </c>
       <c r="E10" s="1">
-        <v>2.54</v>
+        <v>2.27</v>
       </c>
       <c r="F10" s="1">
-        <v>11.03</v>
+        <v>7.69</v>
       </c>
       <c r="G10" s="1">
-        <v>6.7648798040000004</v>
+        <v>5.1034099060000004</v>
       </c>
       <c r="H10" s="1">
-        <v>2.3153459949999999</v>
+        <v>1.532455846</v>
       </c>
       <c r="I10" s="1">
-        <v>5.8435752550000002</v>
+        <v>2.5594885889999999</v>
       </c>
       <c r="K10" s="1">
         <v>772</v>
@@ -22693,28 +22685,28 @@
         <v>18</v>
       </c>
       <c r="B11" s="8">
-        <v>47.175257729999998</v>
+        <v>46.804123709999999</v>
       </c>
       <c r="C11" s="8">
-        <v>392.1443299</v>
+        <v>295.9072165</v>
       </c>
       <c r="D11" s="8">
-        <v>344.96907220000003</v>
+        <v>249.10309280000001</v>
       </c>
       <c r="E11" s="8">
-        <v>2.6391752579999999</v>
+        <v>2.3402061860000001</v>
       </c>
       <c r="F11" s="8">
-        <v>12.48453608</v>
+        <v>8.2474226799999997</v>
       </c>
       <c r="G11" s="8">
-        <v>7.3057515039999998</v>
+        <v>5.321230226</v>
       </c>
       <c r="H11" s="8">
-        <v>2.6335990909999998</v>
+        <v>1.6476098530000001</v>
       </c>
       <c r="I11" s="8">
-        <v>7.6195127749999996</v>
+        <v>3.02126677</v>
       </c>
       <c r="K11" s="8">
         <v>868</v>
@@ -22746,28 +22738,28 @@
         <v>20</v>
       </c>
       <c r="B12" s="6">
-        <v>53.103092779999997</v>
+        <v>52.793814429999998</v>
       </c>
       <c r="C12" s="6">
-        <v>471.32989689999999</v>
+        <v>344.60824739999998</v>
       </c>
       <c r="D12" s="6">
-        <v>418.22680409999998</v>
+        <v>291.81443300000001</v>
       </c>
       <c r="E12" s="6">
-        <v>2.628865979</v>
+        <v>2.3195876289999999</v>
       </c>
       <c r="F12" s="6">
-        <v>13.42268041</v>
+        <v>8.7525773200000003</v>
       </c>
       <c r="G12" s="6">
-        <v>7.8820218970000004</v>
+        <v>5.5314001839999998</v>
       </c>
       <c r="H12" s="6">
-        <v>2.8838130820000001</v>
+        <v>1.7880565479999999</v>
       </c>
       <c r="I12" s="6">
-        <v>9.0837061119999998</v>
+        <v>3.538067093</v>
       </c>
       <c r="K12" s="1">
         <v>964</v>
@@ -22846,28 +22838,28 @@
         <v>6.4991582489999997</v>
       </c>
       <c r="K14" s="8">
-        <v>17.757575760000002</v>
+        <v>70.525252530000003</v>
       </c>
       <c r="L14" s="8">
-        <v>564.47474750000003</v>
+        <v>2249.1414140000002</v>
       </c>
       <c r="M14" s="8">
-        <v>546.71717169999999</v>
+        <v>2178.6161619999998</v>
       </c>
       <c r="N14" s="8">
-        <v>16.171717170000001</v>
+        <v>12.212121209999999</v>
       </c>
       <c r="O14" s="8">
-        <v>42.18181818</v>
+        <v>43.19191919</v>
       </c>
       <c r="P14" s="8">
-        <v>31.917368079999999</v>
+        <v>31.843807160000001</v>
       </c>
       <c r="Q14" s="8">
-        <v>8.2257861139999999</v>
+        <v>8.3447393939999994</v>
       </c>
       <c r="R14" s="8">
-        <v>78.766284540000001</v>
+        <v>79.043439520000007</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -22899,28 +22891,28 @@
         <v>10.81647635</v>
       </c>
       <c r="K15" s="1">
-        <v>28.040816329999998</v>
+        <v>111.2857143</v>
       </c>
       <c r="L15" s="1">
-        <v>1335.9285709999999</v>
+        <v>5308.3979589999999</v>
       </c>
       <c r="M15" s="1">
-        <v>1307.887755</v>
+        <v>5197.1122450000003</v>
       </c>
       <c r="N15" s="1">
-        <v>19.132653059999999</v>
+        <v>14.64285714</v>
       </c>
       <c r="O15" s="1">
-        <v>63.306122449999997</v>
+        <v>64.908163270000003</v>
       </c>
       <c r="P15" s="1">
-        <v>48.346883339999998</v>
+        <v>48.435101549999999</v>
       </c>
       <c r="Q15" s="1">
-        <v>13.25976197</v>
+        <v>13.319270319999999</v>
       </c>
       <c r="R15" s="1">
-        <v>190.4274882</v>
+        <v>190.68622719999999</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -22952,28 +22944,28 @@
         <v>20.597345879999999</v>
       </c>
       <c r="K16" s="8">
-        <v>40.041666669999998</v>
+        <v>159.8125</v>
       </c>
       <c r="L16" s="8">
-        <v>2362.083333</v>
+        <v>9403.4270830000005</v>
       </c>
       <c r="M16" s="8">
-        <v>2322.041667</v>
+        <v>9243.6145830000005</v>
       </c>
       <c r="N16" s="8">
-        <v>21.208333329999999</v>
+        <v>16.208333329999999</v>
       </c>
       <c r="O16" s="8">
-        <v>79.75</v>
+        <v>81.322916669999998</v>
       </c>
       <c r="P16" s="8">
-        <v>60.11468919</v>
+        <v>60.082717520000003</v>
       </c>
       <c r="Q16" s="8">
-        <v>16.91002361</v>
+        <v>16.98016702</v>
       </c>
       <c r="R16" s="8">
-        <v>309.77868050000001</v>
+        <v>308.86185360000002</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
@@ -23005,28 +22997,28 @@
         <v>30.252994170000001</v>
       </c>
       <c r="K17" s="1">
-        <v>49.422680409999998</v>
+        <v>197.3814433</v>
       </c>
       <c r="L17" s="1">
-        <v>3802.6494849999999</v>
+        <v>15126.329900000001</v>
       </c>
       <c r="M17" s="1">
-        <v>3753.2268039999999</v>
+        <v>14928.94845</v>
       </c>
       <c r="N17" s="1">
-        <v>27.391752579999999</v>
+        <v>19.824742270000002</v>
       </c>
       <c r="O17" s="1">
-        <v>99.030927840000004</v>
+        <v>100.8659794</v>
       </c>
       <c r="P17" s="1">
-        <v>78.284567550000006</v>
+        <v>77.986594100000005</v>
       </c>
       <c r="Q17" s="1">
-        <v>20.011952409999999</v>
+        <v>20.336356469999998</v>
       </c>
       <c r="R17" s="1">
-        <v>434.67973760000001</v>
+        <v>447.93002239999998</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
@@ -23034,52 +23026,52 @@
         <v>12</v>
       </c>
       <c r="B18" s="8">
-        <v>11.56565657</v>
+        <v>11.51515152</v>
       </c>
       <c r="C18" s="8">
-        <v>356.18181820000001</v>
+        <v>307.49494950000002</v>
       </c>
       <c r="D18" s="8">
-        <v>344.6161616</v>
+        <v>295.97979800000002</v>
       </c>
       <c r="E18" s="8">
-        <v>18.28282828</v>
+        <v>15.919191919999999</v>
       </c>
       <c r="F18" s="8">
-        <v>38.939393940000002</v>
+        <v>33.272727269999997</v>
       </c>
       <c r="G18" s="8">
-        <v>30.427251779999999</v>
+        <v>26.213870579999998</v>
       </c>
       <c r="H18" s="8">
-        <v>7.4665058220000002</v>
+        <v>6.3452085580000004</v>
       </c>
       <c r="I18" s="8">
-        <v>70.172124819999993</v>
+        <v>50.763472829999998</v>
       </c>
       <c r="K18" s="8">
-        <v>60.878787879999997</v>
+        <v>242.79797980000001</v>
       </c>
       <c r="L18" s="8">
-        <v>5478.181818</v>
+        <v>21825.686870000001</v>
       </c>
       <c r="M18" s="8">
-        <v>5417.30303</v>
+        <v>21582.888889999998</v>
       </c>
       <c r="N18" s="8">
-        <v>28.272727270000001</v>
+        <v>20.979797980000001</v>
       </c>
       <c r="O18" s="8">
-        <v>116.1010101</v>
+        <v>118.01010100000001</v>
       </c>
       <c r="P18" s="8">
-        <v>91.332784939999996</v>
+        <v>91.190876320000001</v>
       </c>
       <c r="Q18" s="8">
-        <v>23.707913600000001</v>
+        <v>23.809413370000001</v>
       </c>
       <c r="R18" s="8">
-        <v>605.69968159999996</v>
+        <v>607.16225970000005</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
@@ -23087,52 +23079,52 @@
         <v>14</v>
       </c>
       <c r="B19" s="1">
-        <v>14.070707069999999</v>
+        <v>14.020202019999999</v>
       </c>
       <c r="C19" s="1">
-        <v>528.08080810000001</v>
+        <v>414.97979800000002</v>
       </c>
       <c r="D19" s="1">
-        <v>514.01010099999996</v>
+        <v>400.95959599999998</v>
       </c>
       <c r="E19" s="1">
-        <v>20.01010101</v>
+        <v>15.969696969999999</v>
       </c>
       <c r="F19" s="1">
-        <v>47.777777780000001</v>
+        <v>37.171717170000001</v>
       </c>
       <c r="G19" s="1">
-        <v>37.322766270000002</v>
+        <v>29.209199430000002</v>
       </c>
       <c r="H19" s="1">
-        <v>9.3793808120000008</v>
+        <v>7.2011670309999998</v>
       </c>
       <c r="I19" s="1">
-        <v>103.10665</v>
+        <v>60.436836079999999</v>
       </c>
       <c r="K19" s="1">
-        <v>72.909090910000003</v>
+        <v>291.17171719999999</v>
       </c>
       <c r="L19" s="1">
-        <v>7488.7474750000001</v>
+        <v>29916.545450000001</v>
       </c>
       <c r="M19" s="1">
-        <v>7415.8383839999997</v>
+        <v>29625.373739999999</v>
       </c>
       <c r="N19" s="1">
-        <v>25.929292929999999</v>
+        <v>20.272727270000001</v>
       </c>
       <c r="O19" s="1">
-        <v>134.05050510000001</v>
+        <v>135.969697</v>
       </c>
       <c r="P19" s="1">
-        <v>103.4549698</v>
+        <v>103.54163389999999</v>
       </c>
       <c r="Q19" s="1">
-        <v>29.003534940000002</v>
+        <v>28.87701839</v>
       </c>
       <c r="R19" s="1">
-        <v>897.39863620000006</v>
+        <v>884.43729010000004</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
@@ -23140,52 +23132,52 @@
         <v>16</v>
       </c>
       <c r="B20" s="8">
-        <v>16.43</v>
+        <v>16.3</v>
       </c>
       <c r="C20" s="8">
-        <v>749.47</v>
+        <v>543.62</v>
       </c>
       <c r="D20" s="8">
-        <v>733.04</v>
+        <v>527.32000000000005</v>
       </c>
       <c r="E20" s="8">
-        <v>23.75</v>
+        <v>17.21</v>
       </c>
       <c r="F20" s="8">
-        <v>58.66</v>
+        <v>42.38</v>
       </c>
       <c r="G20" s="8">
-        <v>45.74794953</v>
+        <v>33.14454963</v>
       </c>
       <c r="H20" s="8">
-        <v>11.76933337</v>
+        <v>8.5527159229999992</v>
       </c>
       <c r="I20" s="8">
-        <v>166.5898833</v>
+        <v>88.030601090000005</v>
       </c>
       <c r="K20" s="8">
-        <v>84.94</v>
+        <v>339.36</v>
       </c>
       <c r="L20" s="8">
-        <v>9726.83</v>
+        <v>38953.08</v>
       </c>
       <c r="M20" s="8">
-        <v>9641.89</v>
+        <v>38613.72</v>
       </c>
       <c r="N20" s="8">
-        <v>26.72</v>
+        <v>17.77</v>
       </c>
       <c r="O20" s="8">
-        <v>149.53</v>
+        <v>151.80000000000001</v>
       </c>
       <c r="P20" s="8">
-        <v>115.5809029</v>
+        <v>115.82207440000001</v>
       </c>
       <c r="Q20" s="8">
-        <v>33.858662119999998</v>
+        <v>33.603654380000002</v>
       </c>
       <c r="R20" s="8">
-        <v>1227.8741</v>
+        <v>1199.4864789999999</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
@@ -23193,52 +23185,52 @@
         <v>18</v>
       </c>
       <c r="B21" s="1">
-        <v>18.24742268</v>
+        <v>18.18556701</v>
       </c>
       <c r="C21" s="1">
-        <v>987.86597940000001</v>
+        <v>692.65979379999999</v>
       </c>
       <c r="D21" s="1">
-        <v>969.6185567</v>
+        <v>674.4742268</v>
       </c>
       <c r="E21" s="1">
-        <v>27</v>
+        <v>19.18556701</v>
       </c>
       <c r="F21" s="1">
-        <v>69.18556701</v>
+        <v>47.927835049999999</v>
       </c>
       <c r="G21" s="1">
-        <v>54.054142400000003</v>
+        <v>37.70811621</v>
       </c>
       <c r="H21" s="1">
-        <v>13.684280660000001</v>
+        <v>9.3981537530000008</v>
       </c>
       <c r="I21" s="1">
-        <v>213.8925749</v>
+        <v>100.1391471</v>
       </c>
       <c r="K21" s="1">
-        <v>93.536082469999997</v>
+        <v>374.12371130000002</v>
       </c>
       <c r="L21" s="1">
-        <v>12308.804120000001</v>
+        <v>49206.164949999998</v>
       </c>
       <c r="M21" s="1">
-        <v>12215.268040000001</v>
+        <v>48832.041239999999</v>
       </c>
       <c r="N21" s="1">
-        <v>29.515463919999998</v>
+        <v>21.958762889999999</v>
       </c>
       <c r="O21" s="1">
-        <v>170.57731960000001</v>
+        <v>172.56701029999999</v>
       </c>
       <c r="P21" s="1">
-        <v>132.63237570000001</v>
+        <v>132.50407939999999</v>
       </c>
       <c r="Q21" s="1">
-        <v>37.083239519999999</v>
+        <v>37.05771867</v>
       </c>
       <c r="R21" s="1">
-        <v>1428.062895</v>
+        <v>1424.5244849999999</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
@@ -23246,52 +23238,52 @@
         <v>20</v>
       </c>
       <c r="B22" s="10">
-        <v>20.40206186</v>
+        <v>20.30927835</v>
       </c>
       <c r="C22" s="10">
-        <v>1256.639175</v>
+        <v>846.8556701</v>
       </c>
       <c r="D22" s="10">
-        <v>1236.2371129999999</v>
+        <v>826.54639180000004</v>
       </c>
       <c r="E22" s="10">
-        <v>29.15463918</v>
+        <v>20.051546389999999</v>
       </c>
       <c r="F22" s="10">
-        <v>79.12371134</v>
+        <v>52.886597940000001</v>
       </c>
       <c r="G22" s="10">
-        <v>61.604193250000002</v>
+        <v>41.392901979999998</v>
       </c>
       <c r="H22" s="10">
-        <v>15.86573351</v>
+        <v>10.517408469999999</v>
       </c>
       <c r="I22" s="10">
-        <v>281.54371459999999</v>
+        <v>123.91606470000001</v>
       </c>
       <c r="K22" s="8">
-        <v>102.7731959</v>
+        <v>410.74226800000002</v>
       </c>
       <c r="L22" s="8">
-        <v>15198.144329999999</v>
+        <v>60834.75258</v>
       </c>
       <c r="M22" s="8">
-        <v>15095.37113</v>
+        <v>60424.010309999998</v>
       </c>
       <c r="N22" s="8">
-        <v>30.618556699999999</v>
+        <v>23.298969069999998</v>
       </c>
       <c r="O22" s="8">
-        <v>190.5257732</v>
+        <v>193.19587630000001</v>
       </c>
       <c r="P22" s="8">
-        <v>148.90385570000001</v>
+        <v>149.11104280000001</v>
       </c>
       <c r="Q22" s="8">
-        <v>41.944222099999998</v>
+        <v>41.5851288</v>
       </c>
       <c r="R22" s="8">
-        <v>1845.465841</v>
+        <v>1801.413258</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
@@ -23537,19 +23529,19 @@
         <v>1</v>
       </c>
       <c r="C28" s="1">
-        <v>413.22222219999998</v>
+        <v>351.68686869999999</v>
       </c>
       <c r="D28" s="1">
-        <v>412.22222219999998</v>
+        <v>350.68686869999999</v>
       </c>
       <c r="E28" s="1">
-        <v>412.22222219999998</v>
+        <v>350.68686869999999</v>
       </c>
       <c r="F28" s="1">
-        <v>412.22222219999998</v>
+        <v>350.68686869999999</v>
       </c>
       <c r="G28" s="1">
-        <v>412.22222219999998</v>
+        <v>350.68686869999999</v>
       </c>
       <c r="H28" s="1">
         <v>0</v>
@@ -23590,19 +23582,19 @@
         <v>1</v>
       </c>
       <c r="C29" s="8">
-        <v>468.71717169999999</v>
+        <v>368.93939390000003</v>
       </c>
       <c r="D29" s="8">
-        <v>467.71717169999999</v>
+        <v>367.93939390000003</v>
       </c>
       <c r="E29" s="8">
-        <v>467.71717169999999</v>
+        <v>367.93939390000003</v>
       </c>
       <c r="F29" s="8">
-        <v>467.71717169999999</v>
+        <v>367.93939390000003</v>
       </c>
       <c r="G29" s="8">
-        <v>467.71717169999999</v>
+        <v>367.93939390000003</v>
       </c>
       <c r="H29" s="8">
         <v>0</v>
@@ -23643,19 +23635,19 @@
         <v>1</v>
       </c>
       <c r="C30" s="1">
-        <v>549.33000000000004</v>
+        <v>401.67</v>
       </c>
       <c r="D30" s="1">
-        <v>548.33000000000004</v>
+        <v>400.67</v>
       </c>
       <c r="E30" s="1">
-        <v>548.33000000000004</v>
+        <v>400.67</v>
       </c>
       <c r="F30" s="1">
-        <v>548.33000000000004</v>
+        <v>400.67</v>
       </c>
       <c r="G30" s="1">
-        <v>548.33000000000004</v>
+        <v>400.67</v>
       </c>
       <c r="H30" s="1">
         <v>0</v>
@@ -23696,19 +23688,19 @@
         <v>1</v>
       </c>
       <c r="C31" s="8">
-        <v>613.0927835</v>
+        <v>425.39175260000002</v>
       </c>
       <c r="D31" s="8">
-        <v>612.0927835</v>
+        <v>424.39175260000002</v>
       </c>
       <c r="E31" s="8">
-        <v>612.0927835</v>
+        <v>424.39175260000002</v>
       </c>
       <c r="F31" s="8">
-        <v>612.0927835</v>
+        <v>424.39175260000002</v>
       </c>
       <c r="G31" s="8">
-        <v>612.0927835</v>
+        <v>424.39175260000002</v>
       </c>
       <c r="H31" s="8">
         <v>0</v>
@@ -23749,19 +23741,19 @@
         <v>1</v>
       </c>
       <c r="C32" s="6">
-        <v>665.18556699999999</v>
+        <v>437.63917529999998</v>
       </c>
       <c r="D32" s="6">
-        <v>664.18556699999999</v>
+        <v>436.63917529999998</v>
       </c>
       <c r="E32" s="6">
-        <v>664.18556699999999</v>
+        <v>436.63917529999998</v>
       </c>
       <c r="F32" s="6">
-        <v>664.18556699999999</v>
+        <v>436.63917529999998</v>
       </c>
       <c r="G32" s="6">
-        <v>664.18556699999999</v>
+        <v>436.63917529999998</v>
       </c>
       <c r="H32" s="6">
         <v>0</v>
@@ -24037,19 +24029,19 @@
         <v>1</v>
       </c>
       <c r="C38" s="8">
-        <v>76.424242419999999</v>
+        <v>65.646464649999999</v>
       </c>
       <c r="D38" s="8">
-        <v>75.424242419999999</v>
+        <v>64.646464649999999</v>
       </c>
       <c r="E38" s="8">
-        <v>75.424242419999999</v>
+        <v>64.646464649999999</v>
       </c>
       <c r="F38" s="8">
-        <v>75.424242419999999</v>
+        <v>64.646464649999999</v>
       </c>
       <c r="G38" s="8">
-        <v>75.424242419999999</v>
+        <v>64.646464649999999</v>
       </c>
       <c r="H38" s="8">
         <v>0</v>
@@ -24090,19 +24082,19 @@
         <v>1</v>
       </c>
       <c r="C39" s="1">
-        <v>98.686868689999997</v>
+        <v>76.858585860000005</v>
       </c>
       <c r="D39" s="1">
-        <v>97.686868689999997</v>
+        <v>75.858585860000005</v>
       </c>
       <c r="E39" s="1">
-        <v>97.686868689999997</v>
+        <v>75.858585860000005</v>
       </c>
       <c r="F39" s="1">
-        <v>97.686868689999997</v>
+        <v>75.858585860000005</v>
       </c>
       <c r="G39" s="1">
-        <v>97.686868689999997</v>
+        <v>75.858585860000005</v>
       </c>
       <c r="H39" s="1">
         <v>0</v>
@@ -24143,19 +24135,19 @@
         <v>1</v>
       </c>
       <c r="C40" s="8">
-        <v>121.93</v>
+        <v>88.94</v>
       </c>
       <c r="D40" s="8">
-        <v>120.93</v>
+        <v>87.94</v>
       </c>
       <c r="E40" s="8">
-        <v>120.93</v>
+        <v>87.94</v>
       </c>
       <c r="F40" s="8">
-        <v>120.93</v>
+        <v>87.94</v>
       </c>
       <c r="G40" s="8">
-        <v>120.93</v>
+        <v>87.94</v>
       </c>
       <c r="H40" s="8">
         <v>0</v>
@@ -24196,19 +24188,19 @@
         <v>1</v>
       </c>
       <c r="C41" s="1">
-        <v>141.8247423</v>
+        <v>99.175257729999998</v>
       </c>
       <c r="D41" s="1">
-        <v>140.8247423</v>
+        <v>98.175257729999998</v>
       </c>
       <c r="E41" s="1">
-        <v>140.8247423</v>
+        <v>98.175257729999998</v>
       </c>
       <c r="F41" s="1">
-        <v>140.8247423</v>
+        <v>98.175257729999998</v>
       </c>
       <c r="G41" s="1">
-        <v>140.8247423</v>
+        <v>98.175257729999998</v>
       </c>
       <c r="H41" s="1">
         <v>0</v>
@@ -24249,19 +24241,19 @@
         <v>1</v>
       </c>
       <c r="C42" s="8">
-        <v>162.95876290000001</v>
+        <v>109.0103093</v>
       </c>
       <c r="D42" s="8">
-        <v>161.95876290000001</v>
+        <v>108.0103093</v>
       </c>
       <c r="E42" s="8">
-        <v>161.95876290000001</v>
+        <v>108.0103093</v>
       </c>
       <c r="F42" s="8">
-        <v>161.95876290000001</v>
+        <v>108.0103093</v>
       </c>
       <c r="G42" s="8">
-        <v>161.95876290000001</v>
+        <v>108.0103093</v>
       </c>
       <c r="H42" s="8">
         <v>0</v>

</xml_diff>